<commit_message>
katilimci exceli oluşturulmalıdır. Otomatik mail atıyor.
</commit_message>
<xml_diff>
--- a/katilimcilar.xlsx
+++ b/katilimcilar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASLAN\PycharmProjects\KatilimBelgesi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3A005F-1B71-465C-B336-49CC1AAC5C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A10D352-814F-43E2-94EB-1EAC6943A96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Bildiri No</t>
   </si>
@@ -59,17 +59,26 @@
     <t>Ammar ASLAN</t>
   </si>
   <si>
-    <t>ammaraslan@gmail.com</t>
+    <t>LORAWAN KABLOSUZ HABERLEŞME PROTOKOLÜNÜN GÜVENLİK ANALİZİ VE LORAWAN TABANLI IOT CİHAZLARINA KARŞI YAPILAN SALDIRILAR</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>A HIGH-PERFORMANCE INTEGER LINEAR PROGRAMMING BASED COMPUTATION FOR TRAFFIC SCHEDULES IN IEEE 802.1 TIME SENSITIVE NETWORKS</t>
+  </si>
+  <si>
+    <t>Selahattin Barış Çelebi</t>
+  </si>
+  <si>
+    <t>ammaraslan@test.com</t>
+  </si>
+  <si>
+    <t>sbariscelebi@test.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="18"/>
       <color theme="1"/>
@@ -109,6 +118,12 @@
       <sz val="18"/>
       <color theme="10"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF555555"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -207,7 +222,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -261,7 +276,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -481,7 +499,7 @@
   <dimension ref="A1:G998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -527,7 +545,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="12">
         <v>44561</v>
@@ -535,18 +553,26 @@
       <c r="E2" s="12">
         <v>44569</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="20" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>13</v>
+      </c>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
+      <c r="F3" s="20" t="s">
+        <v>9</v>
+      </c>
       <c r="G3" s="17"/>
     </row>
     <row r="4" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1957,9 +1983,10 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{E1FBE29D-B2D2-4236-8D56-C2FEAE108834}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{10B957DD-5569-4593-BDF1-485C20452963}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{B711648F-D6D0-45F3-A01B-4D2A0602D31B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>